<commit_message>
assign task to person
</commit_message>
<xml_diff>
--- a/plan/workplan.xlsx
+++ b/plan/workplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9F168F0E-BB47-4473-8F2C-FDB3CFE727EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5B04CEED-D5A1-4AB5-8A73-88E6298D64D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
   <si>
     <t>大分类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,6 +222,16 @@
   <si>
     <t>和前端进行结合，导入之后能在前端表示</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bu</t>
+  </si>
+  <si>
+    <t>bu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fu</t>
   </si>
 </sst>
 </file>
@@ -244,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,17 +301,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -579,7 +596,7 @@
   <dimension ref="A2:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:I13"/>
+      <selection activeCell="E21" sqref="E21:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -595,7 +612,7 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -612,13 +629,13 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
@@ -661,7 +678,9 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
@@ -687,7 +706,9 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>14</v>
       </c>
@@ -713,7 +734,9 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
@@ -739,7 +762,9 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
@@ -767,7 +792,9 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
@@ -793,7 +820,9 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
@@ -819,7 +848,9 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
@@ -849,7 +880,9 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
@@ -875,7 +908,9 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
@@ -901,7 +936,9 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
@@ -927,7 +964,9 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>14</v>
       </c>
@@ -955,7 +994,9 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>14</v>
       </c>
@@ -981,7 +1022,9 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1050,9 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1033,7 +1078,9 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1059,7 +1106,9 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K20" s="1" t="s">
         <v>14</v>
       </c>
@@ -1079,7 +1128,9 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K21" s="1" t="s">
         <v>14</v>
       </c>
@@ -1091,17 +1142,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
     <mergeCell ref="E15:I15"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="E5:I5"/>
@@ -1109,6 +1149,17 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="E9:I9"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
@@ -1135,22 +1186,22 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>